<commit_message>
WIP : Change the naming convention of output automtation result file
</commit_message>
<xml_diff>
--- a/data/Template_competition_analytics.xlsx
+++ b/data/Template_competition_analytics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -277,13 +277,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.66"/>
@@ -425,6 +425,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="https://www.udemy.com/course/snowflake-snowpro-core-certification-exam-questions/?couponCode=KEEPLEARNING"/>

</xml_diff>